<commit_message>
add spu - BNIA nb
</commit_message>
<xml_diff>
--- a/data/open-baltimore/source.xlsx
+++ b/data/open-baltimore/source.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1592E3F3-8004-408D-9697-2B15F6F246B6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>filename</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,23 +111,32 @@
   </si>
   <si>
     <t>https://data.baltimorecity.gov/City-Services/ECB-Citations/ywty-nmtg</t>
+  </si>
+  <si>
+    <t>https://opendata.arcgis.com/datasets/794586676bcc4f5fb629c08c51474cf6_0.geojson</t>
+  </si>
+  <si>
+    <t>Vital Signs 15 Census Demographics</t>
+  </si>
+  <si>
+    <t>extracted the shape of neighborhood defined by BNIA-JFI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -156,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -172,7 +182,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -247,6 +257,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -282,6 +309,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -457,20 +501,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="38.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.25" customWidth="1"/>
+    <col min="1" max="1" width="38.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -489,7 +533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -497,7 +541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -505,7 +549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -513,7 +557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -521,7 +565,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -529,7 +573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -537,7 +581,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -545,7 +589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -553,7 +597,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -561,7 +605,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -569,7 +613,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -577,7 +621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -585,12 +629,23 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add spu - city nb
</commit_message>
<xml_diff>
--- a/data/open-baltimore/source.xlsx
+++ b/data/open-baltimore/source.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1592E3F3-8004-408D-9697-2B15F6F246B6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3065DAE5-35A0-4B72-9623-54DA2C3346CE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>filename</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>extracted the shape of neighborhood defined by BNIA-JFI</t>
+  </si>
+  <si>
+    <t>Neighborhoods.geojson</t>
+  </si>
+  <si>
+    <t>https://data.baltimorecity.gov/Neighborhoods/Neighborhoods/5cni-ybar</t>
+  </si>
+  <si>
+    <t>neighborhood defined by Baltimorecitye as of 2010</t>
   </si>
 </sst>
 </file>
@@ -502,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -648,6 +657,17 @@
         <v>31</v>
       </c>
     </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>